<commit_message>
Added and cleaned tests for ngbd conditions.
</commit_message>
<xml_diff>
--- a/tests/resources/db/Arraignments.xlsx
+++ b/tests/resources/db/Arraignments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
   <si>
     <t>Case</t>
   </si>
@@ -332,13 +332,25 @@
   </si>
   <si>
     <t>4511.20</t>
+  </si>
+  <si>
+    <t>FRA</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -774,19 +786,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="7" width="13.703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,8 +820,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -831,8 +846,11 @@
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="38">
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -854,8 +872,11 @@
       <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="50.7">
+      <c r="H3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -877,8 +898,11 @@
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="50.7">
+      <c r="H4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -900,8 +924,11 @@
       <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="25.35">
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -923,8 +950,11 @@
       <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="38">
+      <c r="H6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -946,8 +976,11 @@
       <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="25.35">
+      <c r="H7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -969,8 +1002,11 @@
       <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="25.35">
+      <c r="H8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -992,8 +1028,11 @@
       <c r="G9" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="38">
+      <c r="H9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
@@ -1015,8 +1054,11 @@
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="50.7">
+      <c r="H10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1038,8 +1080,11 @@
       <c r="G11" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="50.7">
+      <c r="H11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -1061,8 +1106,11 @@
       <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="38">
+      <c r="H12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -1084,8 +1132,11 @@
       <c r="G13" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="25.35">
+      <c r="H13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>73</v>
       </c>
@@ -1107,8 +1158,11 @@
       <c r="G14" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>73</v>
       </c>
@@ -1130,8 +1184,11 @@
       <c r="G15" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="25.35">
+      <c r="H15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>73</v>
       </c>
@@ -1153,8 +1210,11 @@
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
@@ -1176,8 +1236,11 @@
       <c r="G17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="38">
+      <c r="H17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>83</v>
       </c>
@@ -1199,8 +1262,11 @@
       <c r="G18" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="50.7">
+      <c r="H18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>83</v>
       </c>
@@ -1222,8 +1288,11 @@
       <c r="G19" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="50.7">
+      <c r="H19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
@@ -1245,8 +1314,11 @@
       <c r="G20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
@@ -1268,8 +1340,11 @@
       <c r="G21" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="38">
+      <c r="H21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -1291,8 +1366,11 @@
       <c r="G22" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="38">
+      <c r="H22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
@@ -1314,8 +1392,11 @@
       <c r="G23" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="23.45" customHeight="1"/>
+      <c r="H23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>

</xml_diff>